<commit_message>
laser safety snap-on covers; filter wheel servo supplier change to Mouser
</commit_message>
<xml_diff>
--- a/Benchtop-v2/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop-v2/parts-list/Benchtop-partslist-latest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop-v2\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F11223-A916-4988-BBE1-8E88DA1AFEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4570866F-8840-4DEE-ABEF-168E8BC9A8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5652" yWindow="3108" windowWidth="37236" windowHeight="18684" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6888" yWindow="5520" windowWidth="33204" windowHeight="15168" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="461">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -80,46 +80,13 @@
     <t>Detection path</t>
   </si>
   <si>
-    <t>902-0064-000</t>
-  </si>
-  <si>
-    <t>Nodna</t>
-  </si>
-  <si>
     <t>Robotis Dynamixel MX-28R</t>
   </si>
   <si>
     <t>Filter wheel servo</t>
   </si>
   <si>
-    <t>Bought via nodna.de</t>
-  </si>
-  <si>
-    <t>NEW VENDOR NECESSARY!</t>
-  </si>
-  <si>
-    <t>903-0163-100</t>
-  </si>
-  <si>
     <t>Robotis FR07-F101K Set Rotate Bracket (N101 Typ)</t>
-  </si>
-  <si>
-    <t>DX-C4-240</t>
-  </si>
-  <si>
-    <t>(DX-C4-240) Dynamixel DX/RX Cable 4-pin 240mm</t>
-  </si>
-  <si>
-    <t>P00001056</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Playzone </t>
-  </si>
-  <si>
-    <t>YF USB to RS485 Adapter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USB Adapter </t>
   </si>
   <si>
     <t>FISBA READY Beam Bio 488-520-638nm</t>
@@ -1268,9 +1235,6 @@
     <t>3D printed</t>
   </si>
   <si>
-    <t>Todo: laser safety covers for front parts of excitation arms</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -1449,13 +1413,61 @@
   </si>
   <si>
     <t>In many cases a single quad-band detection filter is sufficient, if no strict separation of emission spectra is required. However, manual switching to alignment (no filter) position is cumbersome.</t>
+  </si>
+  <si>
+    <t>Laser safety snap-on covers</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">STL files in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/laser-safety</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> folder</t>
+    </r>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>184-902-0064-000</t>
+  </si>
+  <si>
+    <t>184-903-0163-100</t>
+  </si>
+  <si>
+    <t>USB to RS485 Serial Converter Cable</t>
+  </si>
+  <si>
+    <t>895-USBRS485WE5000BT</t>
+  </si>
+  <si>
+    <t>5-Position filter wheel for 2-inch filters</t>
+  </si>
+  <si>
+    <t>TODO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1585,14 +1597,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1653,6 +1659,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1695,7 +1707,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -1759,7 +1771,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1769,6 +1780,8 @@
     <xf numFmtId="2" fontId="5" fillId="3" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Excel Built-in Heading 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -2158,8 +2171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I90" sqref="I90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2235,18 +2248,18 @@
         <v>12350</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="30" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="D5" s="30">
         <v>0</v>
@@ -2261,7 +2274,7 @@
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
       <c r="I5" s="30" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2272,24 +2285,24 @@
     </row>
     <row r="7" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
@@ -2302,10 +2315,10 @@
         <v>24000</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="41" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -2313,10 +2326,10 @@
         <v>1008062</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D10" s="41">
         <v>0</v>
@@ -2330,15 +2343,15 @@
       </c>
       <c r="G10" s="56"/>
       <c r="I10" s="41" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="41" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="C11" s="41" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="D11" s="41">
         <v>0</v>
@@ -2352,25 +2365,25 @@
       </c>
       <c r="G11" s="56"/>
       <c r="I11" s="41" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
@@ -2383,21 +2396,21 @@
         <v>5254</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D14" s="3">
         <v>1</v>
@@ -2410,18 +2423,18 @@
         <v>520</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B15" s="44" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D15" s="44">
         <v>1</v>
@@ -2429,26 +2442,26 @@
       <c r="E15" s="28">
         <v>1807</v>
       </c>
-      <c r="F15" s="59">
+      <c r="F15" s="58">
         <f t="shared" si="0"/>
         <v>1807</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="I15" s="44" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B16" s="44" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D16" s="44">
         <v>1</v>
@@ -2456,12 +2469,12 @@
       <c r="E16" s="28">
         <v>132</v>
       </c>
-      <c r="F16" s="59">
+      <c r="F16" s="58">
         <f t="shared" si="0"/>
         <v>132</v>
       </c>
       <c r="G16" s="44" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="H16" s="44" t="s">
         <v>13</v>
@@ -2469,13 +2482,13 @@
     </row>
     <row r="17" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B17" s="44" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D17" s="44">
         <v>1</v>
@@ -2483,26 +2496,26 @@
       <c r="E17" s="28">
         <v>250</v>
       </c>
-      <c r="F17" s="59">
+      <c r="F17" s="58">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="I17" s="44" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B18" s="44" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D18" s="44">
         <v>1</v>
@@ -2510,29 +2523,29 @@
       <c r="E18" s="28">
         <v>1807</v>
       </c>
-      <c r="F18" s="59">
+      <c r="F18" s="58">
         <f t="shared" si="0"/>
         <v>1807</v>
       </c>
       <c r="G18" s="44" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="H18" s="44" t="s">
         <v>13</v>
       </c>
       <c r="I18" s="44" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B19" s="44" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D19" s="44">
         <v>1</v>
@@ -2540,26 +2553,26 @@
       <c r="E19" s="28">
         <v>200</v>
       </c>
-      <c r="F19" s="59">
+      <c r="F19" s="58">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="I19" s="44" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="44" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B20" s="44" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D20" s="44">
         <v>1</v>
@@ -2567,26 +2580,26 @@
       <c r="E20" s="28">
         <v>1939</v>
       </c>
-      <c r="F20" s="59">
+      <c r="F20" s="58">
         <f t="shared" si="0"/>
         <v>1939</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="I20" s="44" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D21" s="3">
         <v>1</v>
@@ -2599,21 +2612,21 @@
         <v>110</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
@@ -2626,21 +2639,21 @@
         <v>2450</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
@@ -2653,21 +2666,21 @@
         <v>4800</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D24" s="3">
         <v>1</v>
@@ -2680,28 +2693,28 @@
         <v>870</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="D26" s="3">
         <v>2</v>
@@ -2714,21 +2727,21 @@
         <v>140</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="D27" s="3">
         <v>6</v>
@@ -2741,21 +2754,21 @@
         <v>216</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="58" t="s">
-        <v>439</v>
+      <c r="A28" s="57" t="s">
+        <v>427</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
@@ -2768,21 +2781,21 @@
         <v>43</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="58" t="s">
-        <v>442</v>
+      <c r="A29" s="57" t="s">
+        <v>430</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="D29" s="3">
         <v>1</v>
@@ -2795,21 +2808,21 @@
         <v>29</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="58" t="s">
-        <v>445</v>
+      <c r="A30" s="57" t="s">
+        <v>433</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -2822,21 +2835,21 @@
         <v>195</v>
       </c>
       <c r="G30" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="57" t="s">
+        <v>438</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>437</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="58" t="s">
-        <v>450</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>449</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
@@ -2849,26 +2862,26 @@
         <v>10</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="15" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
     </row>
     <row r="33" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C34" s="3" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D34" s="3">
         <v>1</v>
@@ -2883,20 +2896,20 @@
     </row>
     <row r="36" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D37" s="3">
         <v>2</v>
@@ -2909,21 +2922,21 @@
         <v>1560</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D38" s="3">
         <v>2</v>
@@ -2936,24 +2949,24 @@
         <v>560</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D39" s="3">
         <v>2</v>
@@ -2966,21 +2979,21 @@
         <v>170</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="45" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="B40" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C40" s="45" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="D40" s="44">
         <v>2</v>
@@ -2988,23 +3001,23 @@
       <c r="E40" s="46">
         <v>13</v>
       </c>
-      <c r="F40" s="59">
+      <c r="F40" s="58">
         <f>E40*D40</f>
         <v>26</v>
       </c>
       <c r="H40" s="44" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="45" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="B41" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C41" s="45" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="D41" s="44">
         <v>2</v>
@@ -3012,20 +3025,20 @@
       <c r="E41" s="46">
         <v>18</v>
       </c>
-      <c r="F41" s="59">
+      <c r="F41" s="58">
         <f>E41*D41</f>
         <v>36</v>
       </c>
       <c r="H41" s="44" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D42" s="3">
         <v>1</v>
@@ -3037,13 +3050,13 @@
         <v>30</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -3051,10 +3064,10 @@
         <v>91863</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D43" s="3">
         <v>2</v>
@@ -3067,24 +3080,24 @@
         <v>800</v>
       </c>
       <c r="G43" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="I43" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="50" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="B44" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C44" s="50" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="D44" s="51">
         <v>0</v>
@@ -3092,29 +3105,29 @@
       <c r="E44" s="52">
         <v>656</v>
       </c>
-      <c r="F44" s="60">
+      <c r="F44" s="59">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G44" s="51" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="H44" s="51" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="I44" s="51" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="45" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B45" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C45" s="45" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="D45" s="44">
         <v>2</v>
@@ -3122,26 +3135,26 @@
       <c r="E45" s="46">
         <v>31</v>
       </c>
-      <c r="F45" s="59">
+      <c r="F45" s="58">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="H45" s="44" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="I45" s="44" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="47" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="B46" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C46" s="47" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="D46" s="48">
         <v>10</v>
@@ -3149,26 +3162,26 @@
       <c r="E46" s="49">
         <v>16</v>
       </c>
-      <c r="F46" s="61">
+      <c r="F46" s="60">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
       <c r="H46" s="48" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="I46" s="48" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="47" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="B47" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C47" s="47" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="D47" s="48">
         <v>4</v>
@@ -3176,26 +3189,26 @@
       <c r="E47" s="49">
         <v>41</v>
       </c>
-      <c r="F47" s="61">
+      <c r="F47" s="60">
         <f t="shared" si="1"/>
         <v>164</v>
       </c>
       <c r="H47" s="48" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="I47" s="48" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="45" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="B48" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C48" s="45" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="D48" s="44">
         <v>2</v>
@@ -3203,26 +3216,26 @@
       <c r="E48" s="46">
         <v>99</v>
       </c>
-      <c r="F48" s="59">
+      <c r="F48" s="58">
         <f t="shared" si="1"/>
         <v>198</v>
       </c>
       <c r="H48" s="44" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="I48" s="44" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="47" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="B49" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C49" s="47" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="D49" s="48">
         <v>6</v>
@@ -3230,26 +3243,26 @@
       <c r="E49" s="49">
         <v>189</v>
       </c>
-      <c r="F49" s="61">
+      <c r="F49" s="60">
         <f t="shared" si="1"/>
         <v>1134</v>
       </c>
       <c r="H49" s="48" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="I49" s="48" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="47" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="B50" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C50" s="47" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="D50" s="48">
         <v>6</v>
@@ -3257,26 +3270,26 @@
       <c r="E50" s="49">
         <v>110</v>
       </c>
-      <c r="F50" s="61">
+      <c r="F50" s="60">
         <f t="shared" si="1"/>
         <v>660</v>
       </c>
       <c r="H50" s="48" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="I50" s="48" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="45" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="B51" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C51" s="45" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="D51" s="44">
         <v>4</v>
@@ -3284,26 +3297,26 @@
       <c r="E51" s="46">
         <v>13</v>
       </c>
-      <c r="F51" s="59">
+      <c r="F51" s="58">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="H51" s="44" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="I51" s="44" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="45" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="B52" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C52" s="45" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="D52" s="44">
         <v>2</v>
@@ -3311,23 +3324,23 @@
       <c r="E52" s="46">
         <v>8</v>
       </c>
-      <c r="F52" s="59">
+      <c r="F52" s="58">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="H52" s="44" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="45" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="B53" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C53" s="45" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="D53" s="44">
         <v>4</v>
@@ -3335,26 +3348,26 @@
       <c r="E53" s="46">
         <v>7</v>
       </c>
-      <c r="F53" s="59">
+      <c r="F53" s="58">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="H53" s="44" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="I53" s="44" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="45" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="B54" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C54" s="45" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="D54" s="44">
         <v>6</v>
@@ -3362,26 +3375,26 @@
       <c r="E54" s="46">
         <v>5</v>
       </c>
-      <c r="F54" s="59">
+      <c r="F54" s="58">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="H54" s="44" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="I54" s="44" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="45" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="B55" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C55" s="45" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="D55" s="44">
         <v>4</v>
@@ -3389,26 +3402,26 @@
       <c r="E55" s="46">
         <v>6</v>
       </c>
-      <c r="F55" s="59">
+      <c r="F55" s="58">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="H55" s="44" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="I55" s="44" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="45" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="B56" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C56" s="45" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="D56" s="44">
         <v>4</v>
@@ -3416,26 +3429,26 @@
       <c r="E56" s="46">
         <v>5</v>
       </c>
-      <c r="F56" s="59">
+      <c r="F56" s="58">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="H56" s="44" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="I56" s="44" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="45" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="B57" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C57" s="45" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="D57" s="44">
         <v>2</v>
@@ -3443,23 +3456,23 @@
       <c r="E57" s="46">
         <v>5</v>
       </c>
-      <c r="F57" s="59">
+      <c r="F57" s="58">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="H57" s="44" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="47" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="B58" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C58" s="47" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="D58" s="48">
         <v>2</v>
@@ -3467,26 +3480,26 @@
       <c r="E58" s="49">
         <v>398</v>
       </c>
-      <c r="F58" s="61">
+      <c r="F58" s="60">
         <f t="shared" si="1"/>
         <v>796</v>
       </c>
       <c r="H58" s="48" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="I58" s="48" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="47" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="B59" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C59" s="47" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="D59" s="48">
         <v>2</v>
@@ -3494,26 +3507,26 @@
       <c r="E59" s="49">
         <v>26</v>
       </c>
-      <c r="F59" s="61">
+      <c r="F59" s="60">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="H59" s="48" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="I59" s="48" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="47" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="B60" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C60" s="47" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="D60" s="48">
         <v>2</v>
@@ -3521,26 +3534,26 @@
       <c r="E60" s="49">
         <v>30</v>
       </c>
-      <c r="F60" s="61">
+      <c r="F60" s="60">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="H60" s="48" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="I60" s="48" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="45" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
       <c r="B61" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C61" s="45" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="D61" s="44">
         <v>2</v>
@@ -3548,26 +3561,26 @@
       <c r="E61" s="46">
         <v>36</v>
       </c>
-      <c r="F61" s="59">
+      <c r="F61" s="58">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
       <c r="H61" s="44" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="I61" s="53" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="45" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="B62" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C62" s="45" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="D62" s="44">
         <v>2</v>
@@ -3575,35 +3588,35 @@
       <c r="E62" s="46">
         <v>1757</v>
       </c>
-      <c r="F62" s="59">
+      <c r="F62" s="58">
         <f t="shared" si="1"/>
         <v>3514</v>
       </c>
       <c r="H62" s="44" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="I62" s="53" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
     </row>
     <row r="63" spans="1:9" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="45"/>
       <c r="C63" s="45"/>
       <c r="E63" s="46"/>
-      <c r="F63" s="59"/>
+      <c r="F63" s="58"/>
       <c r="I63" s="53" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="45" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="B64" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C64" s="45" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="D64" s="44">
         <v>2</v>
@@ -3611,24 +3624,24 @@
       <c r="E64" s="46">
         <v>59</v>
       </c>
-      <c r="F64" s="59">
+      <c r="F64" s="58">
         <f>E64*D64</f>
         <v>118</v>
       </c>
       <c r="H64" s="44" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="I64" s="53"/>
     </row>
     <row r="65" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="45" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="B65" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C65" s="45" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="D65" s="44">
         <v>1</v>
@@ -3636,26 +3649,26 @@
       <c r="E65" s="46">
         <v>495</v>
       </c>
-      <c r="F65" s="59">
+      <c r="F65" s="58">
         <f>E65*D65</f>
         <v>495</v>
       </c>
       <c r="H65" s="44" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="I65" s="44" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
     </row>
     <row r="66" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="45" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="B66" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C66" s="45" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="D66" s="44">
         <v>2</v>
@@ -3663,23 +3676,23 @@
       <c r="E66" s="46">
         <v>25</v>
       </c>
-      <c r="F66" s="59">
+      <c r="F66" s="58">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="H66" s="44" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
     </row>
     <row r="67" spans="1:10" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="54" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="B67" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C67" s="45" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="D67" s="44">
         <v>2</v>
@@ -3687,29 +3700,29 @@
       <c r="E67" s="46">
         <v>35</v>
       </c>
-      <c r="F67" s="59">
+      <c r="F67" s="58">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="H67" s="44" t="s">
+        <v>377</v>
+      </c>
+      <c r="I67" s="53" t="s">
         <v>388</v>
       </c>
-      <c r="I67" s="53" t="s">
-        <v>399</v>
-      </c>
       <c r="J67" s="55" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
     </row>
     <row r="68" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="45" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="B68" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C68" s="45" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="D68" s="44">
         <v>2</v>
@@ -3717,83 +3730,86 @@
       <c r="E68" s="46">
         <v>92</v>
       </c>
-      <c r="F68" s="59">
+      <c r="F68" s="58">
         <f t="shared" si="1"/>
         <v>184</v>
       </c>
       <c r="H68" s="44" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="I68" s="44" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="45" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="B69" s="44" t="s">
-        <v>402</v>
-      </c>
-      <c r="C69" s="57" t="s">
-        <v>403</v>
+        <v>391</v>
+      </c>
+      <c r="C69" s="64" t="s">
+        <v>452</v>
       </c>
       <c r="E69" s="46"/>
-      <c r="F69" s="59"/>
+      <c r="F69" s="58"/>
+      <c r="I69" s="44" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="70" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="45"/>
       <c r="C70" s="45"/>
       <c r="E70" s="46"/>
-      <c r="F70" s="59"/>
+      <c r="F70" s="58"/>
     </row>
     <row r="71" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="45"/>
       <c r="C71" s="45"/>
       <c r="E71" s="46"/>
-      <c r="F71" s="59"/>
+      <c r="F71" s="58"/>
     </row>
     <row r="72" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="45"/>
       <c r="C72" s="45"/>
       <c r="E72" s="46"/>
-      <c r="F72" s="59"/>
+      <c r="F72" s="58"/>
     </row>
     <row r="73" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
     </row>
     <row r="74" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="45" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B74" s="44" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C74" s="45" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D74" s="44">
         <v>1</v>
       </c>
       <c r="E74" s="46"/>
-      <c r="F74" s="59"/>
+      <c r="F74" s="58"/>
       <c r="I74" s="44" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
     </row>
     <row r="75" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="45" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="B75" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C75" s="45" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="D75" s="44">
         <v>1</v>
@@ -3801,20 +3817,20 @@
       <c r="E75" s="46">
         <v>63</v>
       </c>
-      <c r="F75" s="59">
+      <c r="F75" s="58">
         <f>D75*E75</f>
         <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="54" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="B76" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C76" s="45" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="D76" s="44">
         <v>2</v>
@@ -3822,20 +3838,20 @@
       <c r="E76" s="46">
         <v>69</v>
       </c>
-      <c r="F76" s="59">
+      <c r="F76" s="58">
         <f>D76*E76</f>
         <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="45" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="B77" s="44" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="C77" s="45" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="D77" s="44">
         <v>1</v>
@@ -3843,63 +3859,63 @@
       <c r="E77" s="46">
         <v>10</v>
       </c>
-      <c r="F77" s="59">
+      <c r="F77" s="58">
         <f>D77*E77</f>
         <v>10</v>
       </c>
       <c r="I77" s="44" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
     </row>
     <row r="78" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="44" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B78" s="44" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C78" s="44" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D78" s="44">
         <v>1</v>
       </c>
       <c r="E78" s="46"/>
-      <c r="F78" s="59"/>
+      <c r="F78" s="58"/>
       <c r="I78" s="44" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
     </row>
     <row r="79" spans="1:10" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
     </row>
     <row r="80" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="s">
-        <v>458</v>
+        <v>446</v>
       </c>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
     </row>
     <row r="81" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="E81" s="9"/>
       <c r="F81" s="9"/>
     </row>
     <row r="82" spans="1:10" s="44" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="45" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="B82" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C82" s="45" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
       <c r="D82" s="44">
         <v>1</v>
@@ -3907,23 +3923,23 @@
       <c r="E82" s="46">
         <v>656</v>
       </c>
-      <c r="F82" s="59">
+      <c r="F82" s="58">
         <f>E82*D82</f>
         <v>656</v>
       </c>
       <c r="I82" s="55" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
     </row>
     <row r="83" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="45" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="B83" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C83" s="45" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
       <c r="D83" s="44">
         <v>1</v>
@@ -3931,20 +3947,20 @@
       <c r="E83" s="46">
         <v>4.6500000000000004</v>
       </c>
-      <c r="F83" s="59">
+      <c r="F83" s="58">
         <f>E83*D83</f>
         <v>4.6500000000000004</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="B84" s="44" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="D84" s="3">
         <v>1</v>
@@ -3952,34 +3968,34 @@
       <c r="E84" s="12">
         <v>4.87</v>
       </c>
-      <c r="F84" s="59">
+      <c r="F84" s="58">
         <f>E84*D84</f>
         <v>4.87</v>
       </c>
     </row>
     <row r="85" spans="1:10" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="s">
-        <v>459</v>
+        <v>447</v>
       </c>
       <c r="E85" s="9"/>
       <c r="F85" s="9"/>
     </row>
     <row r="86" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="E86" s="9"/>
       <c r="F86" s="9"/>
     </row>
     <row r="87" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="D87" s="3">
         <v>1</v>
@@ -3995,24 +4011,19 @@
         <v>13</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I87" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J87" s="4" t="s">
-        <v>19</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="J87" s="4"/>
     </row>
     <row r="88" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>20</v>
+        <v>456</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>15</v>
+        <v>454</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D88" s="3">
         <v>1</v>
@@ -4028,99 +4039,75 @@
         <v>13</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I88" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J88" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="J88" s="4"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>22</v>
+        <v>458</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>15</v>
+        <v>454</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>23</v>
+        <v>457</v>
       </c>
       <c r="D89" s="3">
         <v>1</v>
       </c>
       <c r="E89" s="5">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="F89" s="5">
         <f>E89*D89</f>
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="G89" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I89" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>24</v>
+        <v>392</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>25</v>
+        <v>391</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>26</v>
+        <v>459</v>
       </c>
       <c r="D90" s="3">
         <v>1</v>
       </c>
-      <c r="E90" s="5">
-        <v>12.5</v>
-      </c>
-      <c r="F90" s="5">
-        <f>E90*D90</f>
-        <v>12.5</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H90" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I90" s="3" t="s">
-        <v>27</v>
+      <c r="I90" s="65" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="91" spans="1:10" s="24" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="25" t="s">
-        <v>460</v>
-      </c>
-      <c r="F91" s="62"/>
+        <v>448</v>
+      </c>
+      <c r="F91" s="61"/>
     </row>
     <row r="92" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="24" t="s">
-        <v>463</v>
-      </c>
-      <c r="F92" s="62"/>
+        <v>451</v>
+      </c>
+      <c r="F92" s="61"/>
     </row>
     <row r="93" spans="1:10" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="26" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="D93" s="26">
         <v>1</v>
@@ -4128,17 +4115,17 @@
       <c r="E93" s="28">
         <v>189</v>
       </c>
-      <c r="F93" s="63"/>
+      <c r="F93" s="62"/>
     </row>
     <row r="94" spans="1:10" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="26" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C94" s="26" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="D94" s="26">
         <v>1</v>
@@ -4146,17 +4133,17 @@
       <c r="E94" s="28">
         <v>37</v>
       </c>
-      <c r="F94" s="63"/>
+      <c r="F94" s="62"/>
     </row>
     <row r="95" spans="1:10" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="26" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="B95" s="26" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="D95" s="26">
         <v>2</v>
@@ -4164,17 +4151,17 @@
       <c r="E95" s="28">
         <v>4.7300000000000004</v>
       </c>
-      <c r="F95" s="63"/>
+      <c r="F95" s="62"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="B96" s="26" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="D96" s="3">
         <v>1</v>
@@ -4185,13 +4172,13 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="B97" s="26" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="D97" s="3">
         <v>1</v>
@@ -4202,13 +4189,13 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="B98" s="26" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="D98" s="3">
         <v>1</v>
@@ -4219,25 +4206,25 @@
     </row>
     <row r="99" spans="1:9" s="24" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="25" t="s">
-        <v>266</v>
-      </c>
-      <c r="F99" s="62"/>
+        <v>255</v>
+      </c>
+      <c r="F99" s="61"/>
     </row>
     <row r="100" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="24" t="s">
-        <v>267</v>
-      </c>
-      <c r="F100" s="62"/>
+        <v>256</v>
+      </c>
+      <c r="F100" s="61"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D101" s="3">
         <v>1</v>
@@ -4253,18 +4240,18 @@
         <v>13</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="41" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B102" s="41" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C102" s="41" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D102" s="41">
         <v>0</v>
@@ -4280,18 +4267,18 @@
         <v>13</v>
       </c>
       <c r="I102" s="41" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="103" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="41" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B103" s="41" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C103" s="41" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D103" s="41">
         <v>0</v>
@@ -4307,18 +4294,18 @@
         <v>13</v>
       </c>
       <c r="I103" s="41" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="41" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B104" s="41" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C104" s="41" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D104" s="41">
         <v>0</v>
@@ -4334,18 +4321,18 @@
         <v>13</v>
       </c>
       <c r="I104" s="41" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="105" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="41" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B105" s="41" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C105" s="41" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D105" s="41">
         <v>0</v>
@@ -4361,18 +4348,18 @@
         <v>13</v>
       </c>
       <c r="I105" s="41" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="41" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B106" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C106" s="41" t="s">
         <v>71</v>
-      </c>
-      <c r="C106" s="41" t="s">
-        <v>82</v>
       </c>
       <c r="D106" s="41">
         <v>0</v>
@@ -4388,25 +4375,25 @@
         <v>13</v>
       </c>
       <c r="I106" s="41" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="107" spans="1:9" s="33" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A107" s="32" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="E107" s="34"/>
       <c r="F107" s="34"/>
     </row>
     <row r="108" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="37" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="B108" s="35" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="C108" s="39" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="D108" s="35">
         <v>1</v>
@@ -4422,10 +4409,10 @@
         <v>13</v>
       </c>
       <c r="H108" s="35" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="I108" s="35" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -4433,10 +4420,10 @@
         <v>11454</v>
       </c>
       <c r="B109" s="35" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="D109" s="3">
         <v>0</v>
@@ -4452,10 +4439,10 @@
         <v>13</v>
       </c>
       <c r="H109" s="35" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -4463,10 +4450,10 @@
         <v>11044</v>
       </c>
       <c r="B110" s="35" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="C110" s="40" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D110" s="3">
         <v>0</v>
@@ -4482,21 +4469,21 @@
         <v>13</v>
       </c>
       <c r="H110" s="35" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="B111" s="35" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="C111" s="40" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="D111" s="3">
         <v>0</v>
@@ -4512,21 +4499,21 @@
         <v>13</v>
       </c>
       <c r="H111" s="35" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="B112" s="35" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="C112" s="40" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="D112" s="3">
         <v>0</v>
@@ -4542,12 +4529,12 @@
         <v>13</v>
       </c>
       <c r="H112" s="35" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="113" spans="1:6" s="33" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A113" s="32" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="E113" s="34"/>
       <c r="F113" s="34"/>
@@ -4602,20 +4589,20 @@
     </row>
     <row r="131" spans="1:9" s="7" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E131" s="9"/>
       <c r="F131" s="9"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D132" s="3">
         <v>1</v>
@@ -4628,21 +4615,21 @@
         <v>3582</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="D133" s="3">
         <v>1</v>
@@ -4655,21 +4642,21 @@
         <v>1630</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="I133" s="3" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="D134" s="3">
         <v>1</v>
@@ -4682,21 +4669,21 @@
         <v>886</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="I134" s="3" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="D135" s="3">
         <v>1</v>
@@ -4709,21 +4696,21 @@
         <v>163</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="I135" s="3" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D136" s="3">
         <v>1</v>
@@ -4736,18 +4723,18 @@
         <v>11</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D137" s="3">
         <v>1</v>
@@ -4760,18 +4747,18 @@
         <v>520</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="D138" s="3">
         <v>1</v>
@@ -4784,18 +4771,18 @@
         <v>193</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="139" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="41" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B139" s="41" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C139" s="41" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D139" s="41">
         <v>0</v>
@@ -4808,21 +4795,21 @@
         <v>0</v>
       </c>
       <c r="G139" s="41" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="I139" s="41" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="140" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="41" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="B140" s="41" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="C140" s="41" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="D140" s="41">
         <v>16</v>
@@ -4835,15 +4822,15 @@
         <v>160</v>
       </c>
       <c r="G140" s="41" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="I140" s="41" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
     </row>
     <row r="144" spans="1:9" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="8" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C144" s="7"/>
       <c r="E144" s="18"/>
@@ -4851,13 +4838,13 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D145" s="3">
         <v>1</v>
@@ -4872,13 +4859,13 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D146" s="3">
         <v>1</v>
@@ -4893,13 +4880,13 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D147" s="3">
         <v>1</v>
@@ -4914,13 +4901,13 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D148" s="3">
         <v>1</v>
@@ -4935,13 +4922,13 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D149" s="3">
         <v>1</v>
@@ -4956,13 +4943,13 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B150" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C150" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="C150" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="D150" s="3">
         <v>1</v>
@@ -4977,13 +4964,13 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D151" s="3">
         <v>1</v>
@@ -4998,13 +4985,13 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D152" s="3">
         <v>1</v>
@@ -5019,13 +5006,13 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D153" s="3">
         <v>1</v>
@@ -5040,13 +5027,13 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D154" s="3">
         <v>2</v>
@@ -5061,13 +5048,13 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D155" s="3">
         <v>1</v>
@@ -5080,18 +5067,18 @@
         <v>304.75</v>
       </c>
       <c r="I155" s="3" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D156" s="3">
         <v>1</v>
@@ -5104,18 +5091,18 @@
         <v>148.21</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D157" s="3">
         <v>1</v>
@@ -5128,18 +5115,18 @@
         <v>348.45</v>
       </c>
       <c r="I157" s="3" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="D158" s="3">
         <v>1</v>
@@ -5154,13 +5141,13 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D159" s="3">
         <v>1</v>
@@ -5173,18 +5160,18 @@
         <v>34.5</v>
       </c>
       <c r="I159" s="3" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="D160" s="3">
         <v>1</v>
@@ -5197,18 +5184,18 @@
         <v>51.45</v>
       </c>
       <c r="I160" s="3" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D161" s="3">
         <v>2</v>
@@ -5223,13 +5210,13 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D162" s="3">
         <v>1</v>
@@ -5244,13 +5231,13 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="D163" s="3">
         <v>2</v>
@@ -5263,18 +5250,18 @@
         <v>81.02</v>
       </c>
       <c r="I163" s="3" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D164" s="3">
         <v>2</v>
@@ -5287,18 +5274,18 @@
         <v>167.19623200000001</v>
       </c>
       <c r="I164" s="3" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D165" s="3">
         <v>4</v>
@@ -5311,18 +5298,18 @@
         <v>280.416</v>
       </c>
       <c r="I165" s="3" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D166" s="3">
         <v>2</v>
@@ -5335,18 +5322,18 @@
         <v>57.5</v>
       </c>
       <c r="I166" s="4" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D167" s="3">
         <v>2</v>
@@ -5361,10 +5348,10 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B168" s="3" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="D168" s="3">
         <v>1</v>
@@ -5377,15 +5364,15 @@
         <v>205</v>
       </c>
       <c r="I168" s="3" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B169" s="3" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="D169" s="3">
         <v>2</v>
@@ -5398,7 +5385,7 @@
         <v>24</v>
       </c>
       <c r="I169" s="3" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="170" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -5408,19 +5395,19 @@
     </row>
     <row r="171" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A171" s="8" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="F171" s="9"/>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="D172" s="3">
         <v>4</v>
@@ -5433,18 +5420,18 @@
         <v>66</v>
       </c>
       <c r="I172" s="3" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D173" s="3">
         <v>4</v>
@@ -5457,18 +5444,18 @@
         <v>29.88</v>
       </c>
       <c r="I173" s="3" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D174" s="3">
         <v>2</v>
@@ -5481,18 +5468,18 @@
         <v>280</v>
       </c>
       <c r="I174" s="3" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D175" s="3">
         <v>1</v>
@@ -5505,18 +5492,18 @@
         <v>438</v>
       </c>
       <c r="I175" s="3" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D176" s="3">
         <v>1</v>
@@ -5531,13 +5518,13 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D177" s="3">
         <v>1</v>
@@ -5550,18 +5537,18 @@
         <v>914</v>
       </c>
       <c r="I177" s="3" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="D178" s="3">
         <v>2</v>
@@ -5574,18 +5561,18 @@
         <v>36</v>
       </c>
       <c r="I178" s="3" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D179" s="3">
         <v>4</v>
@@ -5600,13 +5587,13 @@
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="D180" s="3">
         <v>10</v>
@@ -5621,13 +5608,13 @@
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D181" s="3">
         <v>10</v>
@@ -5642,13 +5629,13 @@
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D182" s="3">
         <v>6</v>
@@ -5663,13 +5650,13 @@
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="D183" s="3">
         <v>2</v>
@@ -5682,18 +5669,18 @@
         <v>64</v>
       </c>
       <c r="I183" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="D184" s="3">
         <v>1</v>
@@ -5706,18 +5693,18 @@
         <v>25</v>
       </c>
       <c r="I184" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="D185" s="3">
         <v>2</v>
@@ -5732,13 +5719,13 @@
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="D186" s="3">
         <v>1</v>
@@ -5751,18 +5738,18 @@
         <v>60</v>
       </c>
       <c r="I186" s="3" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D187" s="3">
         <v>1</v>
@@ -5777,13 +5764,13 @@
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="D188" s="3">
         <v>1</v>
@@ -5798,13 +5785,13 @@
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="D189" s="3">
         <v>1</v>
@@ -5819,13 +5806,13 @@
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="D190" s="3">
         <v>1</v>
@@ -5840,13 +5827,13 @@
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D191" s="3">
         <v>1</v>
@@ -5861,13 +5848,13 @@
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="D192" s="3">
         <v>2</v>
@@ -5882,13 +5869,13 @@
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="D193" s="3">
         <v>2</v>
@@ -5903,13 +5890,13 @@
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="D194" s="3">
         <v>1</v>
@@ -5924,13 +5911,13 @@
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D195" s="3">
         <v>1</v>
@@ -5945,13 +5932,13 @@
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D196" s="3">
         <v>2</v>
@@ -5966,7 +5953,7 @@
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C197" s="3" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="D197" s="3">
         <v>4</v>
@@ -5974,7 +5961,7 @@
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C198" s="3" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="D198" s="3">
         <v>10</v>
@@ -5982,18 +5969,18 @@
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C199" s="3" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="D199" s="3">
         <v>1</v>
       </c>
       <c r="I199" s="3" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C200" s="3" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="D200" s="3">
         <v>1</v>
@@ -6001,7 +5988,7 @@
     </row>
     <row r="204" spans="1:11" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A204" s="8" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="C204" s="7"/>
       <c r="E204" s="18"/>
@@ -6009,225 +5996,225 @@
     </row>
     <row r="205" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B205" s="3" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C205" s="19" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="D205" s="3">
         <v>1</v>
       </c>
       <c r="G205" s="3" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="I205" s="3" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="J205" s="3" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="K205" s="4"/>
     </row>
     <row r="206" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B206" s="3" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C206" s="19" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="D206" s="3">
         <v>1</v>
       </c>
       <c r="G206" s="3" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="I206" s="3" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="J206" s="3" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="K206" s="4"/>
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B207" s="3" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C207" s="19" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="D207" s="3">
         <v>2</v>
       </c>
       <c r="G207" s="3" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="I207" s="3" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="J207" s="3" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B208" s="3" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="D208" s="3">
         <v>1</v>
       </c>
       <c r="G208" s="3" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="J208" s="3" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B209" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C209" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="D209" s="3">
+        <v>1</v>
+      </c>
+      <c r="G209" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="J209" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="C209" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="D209" s="3">
-        <v>1</v>
-      </c>
-      <c r="G209" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="J209" s="3" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C210" s="19" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D210" s="3">
         <v>0</v>
       </c>
       <c r="G210" s="3" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="I210" s="3" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="J210" s="19" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B211" s="3" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C211" s="19" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D211" s="3">
         <v>2</v>
       </c>
       <c r="G211" s="3" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="I211" s="3" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="J211" s="19" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B212" s="3" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C212" s="19" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="D212" s="3">
         <v>2</v>
       </c>
       <c r="G212" s="3" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="I212" s="3" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="J212" s="19" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B213" s="3" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="D213" s="3">
         <v>1</v>
       </c>
       <c r="G213" s="3" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="J213" s="3" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="214" spans="1:11" s="20" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A214" s="20" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="B214" s="19" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C214" s="19" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="D214" s="19">
         <v>10</v>
       </c>
-      <c r="F214" s="64"/>
+      <c r="F214" s="63"/>
       <c r="G214" s="19" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="I214" s="4" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="J214" s="19" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="215" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B215" s="19" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C215" s="19" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="D215" s="3">
         <v>2</v>
       </c>
       <c r="G215" s="3" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="J215" s="3" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="K215" s="4"/>
     </row>
     <row r="216" spans="1:11" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B216" s="3" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="D216" s="3">
         <v>1</v>
@@ -6235,18 +6222,18 @@
       <c r="E216" s="22"/>
       <c r="F216" s="22"/>
       <c r="G216" s="3" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="J216" s="21" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="217" spans="1:11" s="21" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B217" s="3" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="D217" s="3">
         <v>1</v>
@@ -6254,45 +6241,45 @@
       <c r="E217" s="22"/>
       <c r="F217" s="22"/>
       <c r="G217" s="3" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="J217" s="21" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B218" s="3" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="D218" s="3">
         <v>1</v>
       </c>
       <c r="G218" s="3" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="I218" s="3" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="J218" s="3" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="220" spans="1:11" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A220" s="8" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E220" s="9"/>
       <c r="F220" s="9"/>
     </row>
     <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B221" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="D221" s="3">
         <v>0</v>
@@ -6305,15 +6292,15 @@
         <v>0</v>
       </c>
       <c r="I221" s="3" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B222" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="D222" s="3">
         <v>0</v>
@@ -6328,10 +6315,10 @@
     </row>
     <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B223" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="D223" s="3">
         <v>0</v>
@@ -6344,15 +6331,15 @@
         <v>0</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B224" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="D224" s="3">
         <v>0</v>
@@ -6367,10 +6354,10 @@
     </row>
     <row r="225" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B225" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="D225" s="3">
         <v>0</v>
@@ -6385,10 +6372,10 @@
     </row>
     <row r="226" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B226" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="D226" s="3">
         <v>0</v>
@@ -6403,10 +6390,10 @@
     </row>
     <row r="227" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B227" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="D227" s="3">
         <v>0</v>
@@ -6421,10 +6408,10 @@
     </row>
     <row r="228" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B228" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="D228" s="3">
         <v>0</v>
@@ -6439,10 +6426,10 @@
     </row>
     <row r="229" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B229" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="D229" s="3">
         <v>0</v>
@@ -6457,10 +6444,10 @@
     </row>
     <row r="230" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B230" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C230" s="3" t="s">
         <v>247</v>
-      </c>
-      <c r="C230" s="3" t="s">
-        <v>258</v>
       </c>
       <c r="D230" s="3">
         <v>6</v>
@@ -6475,10 +6462,10 @@
     </row>
     <row r="231" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B231" s="3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="D231" s="3">
         <v>10</v>
@@ -6491,16 +6478,16 @@
         <v>1215</v>
       </c>
       <c r="I231" s="3" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="234" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E234" s="23" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="F234" s="5">
         <f>SUM(F3:F232)</f>
-        <v>101295.21398799999</v>
+        <v>101317.71398799999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>